<commit_message>
fixing inputs to server
</commit_message>
<xml_diff>
--- a/tests/data/proteins/MQ_pdata.xlsx
+++ b/tests/data/proteins/MQ_pdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MQoutput\txt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\omicscope\omicscope\tests\data\proteins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B07BFE-45AF-44C1-87DF-F49389924CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED450B-967A-45AB-9BDF-28071DC0BE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{83313E20-614E-41FA-98F0-5A02D9BB86A3}"/>
   </bookViews>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Biological</t>
-  </si>
-  <si>
-    <t>TechRep</t>
   </si>
   <si>
     <t>Condition</t>
@@ -121,8 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +438,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,164 +446,132 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>